<commit_message>
Commit 0.0.1 generated artifacts
</commit_message>
<xml_diff>
--- a/project/excel/gocam.xlsx
+++ b/project/excel/gocam.xlsx
@@ -1,35 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Model" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Activity" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EvidenceItem" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CausalAssociation" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MolecularFunctionAssociation" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BiologicalProcessAssociation" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CellularAnatomicalEntityAssociation" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MoleculeAssociation" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Object" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PublicationObject" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EvidenceTermObject" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MolecularFunctionTermObject" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BiologicalProcessTermObject" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CellularAnatomicalEntityTermObject" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MoleculeTermObject" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CellTypeTermObject" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GrossAnatomicalStructureTermObject" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PhaseTermObject" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GeneProductTermObject" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ProteinComplexTermObject" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TaxonTermObject" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PredicateTermObject" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ProvenanceInfo" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="Model" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Activity" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="EvidenceItem" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="CausalAssociation" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="MolecularFunctionAssociation" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="BiologicalProcessAssociation" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="CellularAnatomicalEntityAssociation" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="CellTypeAssociation" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="GrossAnatomyAssociation" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="MoleculeAssociation" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Object" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="PublicationObject" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="EvidenceTermObject" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="MolecularFunctionTermObject" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="BiologicalProcessTermObject" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="CellularAnatomicalEntityTermObject" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="MoleculeTermObject" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="CellTypeTermObject" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="GrossAnatomicalStructureTermObject" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="PhaseTermObject" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="GeneProductTermObject" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="ProteinComplexTermObject" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="TaxonTermObject" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="PredicateTermObject" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="ProvenanceInfo" sheetId="25" state="visible" r:id="rId25"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -501,6 +503,88 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>term</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>evidence</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>provenances</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>obsolete</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -546,7 +630,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -587,7 +671,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -628,7 +712,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -669,7 +753,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -710,7 +794,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -751,7 +835,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -792,7 +876,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -833,13 +917,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -855,6 +939,67 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>enabled_by</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>molecular_function</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>occurs_in</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>part_of</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>has_direct_input</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>causal_associations</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>provenances</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>label</t>
         </is>
       </c>
@@ -874,7 +1019,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -915,13 +1060,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -937,36 +1082,226 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>enabled_by</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>molecular_function</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>occurs_in</t>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>obsolete</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>obsolete</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>obsolete</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>contributor</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>created</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>provided_by</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>term</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>reference</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>with_objects</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>provenances</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>predicate</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>downstream_activity</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>evidence</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>part_of</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>has_direct_input</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>causal_associations</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
           <t>provenances</t>
         </is>
       </c>
@@ -976,171 +1311,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>obsolete</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>obsolete</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>obsolete</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>contributor</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>created</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>date</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>provided_by</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1162,12 +1333,12 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>reference</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>with_objects</t>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>evidence</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -1181,42 +1352,37 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>predicate</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>downstream_activity</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>term</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
         <is>
           <t>evidence</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>provenances</t>
         </is>
@@ -1227,7 +1393,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1268,7 +1434,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1309,7 +1475,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1348,86 +1514,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>term</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>evidence</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>provenances</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>obsolete</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>